<commit_message>
Completing Using QFile for Notes Dialog
Other things that's in this commit:
~ Edited the Week 11 Gantt Chart to remove the hidden rows in the middle of it
- Removing actions from the Top Menu Bar that we are not using
+ Adding actions to the Top Menu Bar that we are using. Import and Export's functionality is not finished yet.
~ Changing the "About" menu option's test to be more accurate.
+ Adding a function to toggle the Admin Functions to be either "Enabled" or "Disabled"
+ Adding Placeholder UI for our previous features
</commit_message>
<xml_diff>
--- a/Week 11 Gantt Chart.xlsx
+++ b/Week 11 Gantt Chart.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B278C59-F309-406D-A93F-EF1CA165E78F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{3B278C59-F309-406D-A93F-EF1CA165E78F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1051450C-DC44-4B11-9197-901ED253898C}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="51">
   <si>
     <t>Project Start:</t>
   </si>
@@ -164,9 +164,6 @@
     <t xml:space="preserve"> CIS 227 C++2, Section 5660, Winter 2023 Semester, Group 4 </t>
   </si>
   <si>
-    <t>Chris</t>
-  </si>
-  <si>
     <t>Jacob</t>
   </si>
   <si>
@@ -185,9 +182,6 @@
     <t>Team Lead</t>
   </si>
   <si>
-    <t>Gantt Chart</t>
-  </si>
-  <si>
     <t>Documentation</t>
   </si>
   <si>
@@ -203,9 +197,6 @@
     <t>Project Lead For The Week:   Chris R.</t>
   </si>
   <si>
-    <t>Front-End</t>
-  </si>
-  <si>
     <t>Use Qfile for notes dialog</t>
   </si>
   <si>
@@ -233,7 +224,10 @@
     <t>Begin new feature</t>
   </si>
   <si>
-    <t xml:space="preserve">Back-End </t>
+    <t>UX/UI Programmer</t>
+  </si>
+  <si>
+    <t>Functional Programmer</t>
   </si>
 </sst>
 </file>
@@ -882,9 +876,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="12" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="7" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -910,6 +901,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1476,11 +1470,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:BL41"/>
+  <dimension ref="A1:BL30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B40" sqref="B40"/>
+      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1524,37 +1518,37 @@
       <c r="A3" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="80" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" s="85" t="s">
+      <c r="B3" s="79" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="84" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="86"/>
-      <c r="E3" s="84">
+      <c r="D3" s="85"/>
+      <c r="E3" s="83">
         <v>44951</v>
       </c>
-      <c r="F3" s="84"/>
+      <c r="F3" s="83"/>
       <c r="I3" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
-      <c r="L3" s="87" t="s">
+      <c r="L3" s="86" t="s">
+        <v>32</v>
+      </c>
+      <c r="M3" s="86"/>
+      <c r="N3" s="86"/>
+      <c r="O3" s="86"/>
+      <c r="P3" s="86"/>
+      <c r="R3" s="87" t="s">
         <v>33</v>
       </c>
-      <c r="M3" s="87"/>
-      <c r="N3" s="87"/>
-      <c r="O3" s="87"/>
-      <c r="P3" s="87"/>
-      <c r="R3" s="88" t="s">
-        <v>34</v>
-      </c>
-      <c r="S3" s="88"/>
-      <c r="T3" s="88"/>
-      <c r="U3" s="88"/>
-      <c r="V3" s="88"/>
-      <c r="W3" s="79"/>
+      <c r="S3" s="87"/>
+      <c r="T3" s="87"/>
+      <c r="U3" s="87"/>
+      <c r="V3" s="87"/>
+      <c r="W3" s="88"/>
       <c r="Y3" s="3"/>
       <c r="Z3" s="3"/>
       <c r="AA3" s="3"/>
@@ -1564,94 +1558,94 @@
       <c r="A4" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="80"/>
-      <c r="C4" s="85" t="s">
+      <c r="B4" s="79"/>
+      <c r="C4" s="84" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="86"/>
+      <c r="D4" s="85"/>
       <c r="E4" s="7">
         <v>10</v>
       </c>
-      <c r="I4" s="81">
+      <c r="I4" s="80">
         <f>I5</f>
         <v>45012</v>
       </c>
-      <c r="J4" s="82"/>
-      <c r="K4" s="82"/>
-      <c r="L4" s="82"/>
-      <c r="M4" s="82"/>
-      <c r="N4" s="82"/>
-      <c r="O4" s="83"/>
-      <c r="P4" s="81">
+      <c r="J4" s="81"/>
+      <c r="K4" s="81"/>
+      <c r="L4" s="81"/>
+      <c r="M4" s="81"/>
+      <c r="N4" s="81"/>
+      <c r="O4" s="82"/>
+      <c r="P4" s="80">
         <f>P5</f>
         <v>45019</v>
       </c>
-      <c r="Q4" s="82"/>
-      <c r="R4" s="82"/>
-      <c r="S4" s="82"/>
-      <c r="T4" s="82"/>
-      <c r="U4" s="82"/>
-      <c r="V4" s="83"/>
-      <c r="W4" s="81">
+      <c r="Q4" s="81"/>
+      <c r="R4" s="81"/>
+      <c r="S4" s="81"/>
+      <c r="T4" s="81"/>
+      <c r="U4" s="81"/>
+      <c r="V4" s="82"/>
+      <c r="W4" s="80">
         <f>W5</f>
         <v>45026</v>
       </c>
-      <c r="X4" s="82"/>
-      <c r="Y4" s="82"/>
-      <c r="Z4" s="82"/>
-      <c r="AA4" s="82"/>
-      <c r="AB4" s="82"/>
-      <c r="AC4" s="83"/>
-      <c r="AD4" s="81">
+      <c r="X4" s="81"/>
+      <c r="Y4" s="81"/>
+      <c r="Z4" s="81"/>
+      <c r="AA4" s="81"/>
+      <c r="AB4" s="81"/>
+      <c r="AC4" s="82"/>
+      <c r="AD4" s="80">
         <f>AD5</f>
         <v>45033</v>
       </c>
-      <c r="AE4" s="82"/>
-      <c r="AF4" s="82"/>
-      <c r="AG4" s="82"/>
-      <c r="AH4" s="82"/>
-      <c r="AI4" s="82"/>
-      <c r="AJ4" s="83"/>
-      <c r="AK4" s="81">
+      <c r="AE4" s="81"/>
+      <c r="AF4" s="81"/>
+      <c r="AG4" s="81"/>
+      <c r="AH4" s="81"/>
+      <c r="AI4" s="81"/>
+      <c r="AJ4" s="82"/>
+      <c r="AK4" s="80">
         <f>AK5</f>
         <v>45040</v>
       </c>
-      <c r="AL4" s="82"/>
-      <c r="AM4" s="82"/>
-      <c r="AN4" s="82"/>
-      <c r="AO4" s="82"/>
-      <c r="AP4" s="82"/>
-      <c r="AQ4" s="83"/>
-      <c r="AR4" s="81">
+      <c r="AL4" s="81"/>
+      <c r="AM4" s="81"/>
+      <c r="AN4" s="81"/>
+      <c r="AO4" s="81"/>
+      <c r="AP4" s="81"/>
+      <c r="AQ4" s="82"/>
+      <c r="AR4" s="80">
         <f>AR5</f>
         <v>45047</v>
       </c>
-      <c r="AS4" s="82"/>
-      <c r="AT4" s="82"/>
-      <c r="AU4" s="82"/>
-      <c r="AV4" s="82"/>
-      <c r="AW4" s="82"/>
-      <c r="AX4" s="83"/>
-      <c r="AY4" s="81">
+      <c r="AS4" s="81"/>
+      <c r="AT4" s="81"/>
+      <c r="AU4" s="81"/>
+      <c r="AV4" s="81"/>
+      <c r="AW4" s="81"/>
+      <c r="AX4" s="82"/>
+      <c r="AY4" s="80">
         <f>AY5</f>
         <v>45054</v>
       </c>
-      <c r="AZ4" s="82"/>
-      <c r="BA4" s="82"/>
-      <c r="BB4" s="82"/>
-      <c r="BC4" s="82"/>
-      <c r="BD4" s="82"/>
-      <c r="BE4" s="83"/>
-      <c r="BF4" s="81">
+      <c r="AZ4" s="81"/>
+      <c r="BA4" s="81"/>
+      <c r="BB4" s="81"/>
+      <c r="BC4" s="81"/>
+      <c r="BD4" s="81"/>
+      <c r="BE4" s="82"/>
+      <c r="BF4" s="80">
         <f>BF5</f>
         <v>45061</v>
       </c>
-      <c r="BG4" s="82"/>
-      <c r="BH4" s="82"/>
-      <c r="BI4" s="82"/>
-      <c r="BJ4" s="82"/>
-      <c r="BK4" s="82"/>
-      <c r="BL4" s="83"/>
+      <c r="BG4" s="81"/>
+      <c r="BH4" s="81"/>
+      <c r="BI4" s="81"/>
+      <c r="BJ4" s="81"/>
+      <c r="BK4" s="81"/>
+      <c r="BL4" s="82"/>
     </row>
     <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="54" t="s">
@@ -2026,7 +2020,7 @@
         <v>21</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="C8" s="63"/>
       <c r="D8" s="18"/>
@@ -2034,7 +2028,7 @@
       <c r="F8" s="20"/>
       <c r="G8" s="16"/>
       <c r="H8" s="16" t="str">
-        <f t="shared" ref="H8:H34" si="3">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="H8:H23" si="3">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
       <c r="I8" s="39"/>
@@ -2099,10 +2093,10 @@
         <v>26</v>
       </c>
       <c r="B9" s="73" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C9" s="64" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D9" s="21">
         <v>0</v>
@@ -2175,15 +2169,15 @@
       <c r="BK9" s="39"/>
       <c r="BL9" s="39"/>
     </row>
-    <row r="10" spans="1:64" s="3" customFormat="1" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="54" t="s">
         <v>22</v>
       </c>
       <c r="B10" s="73" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C10" s="64" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D10" s="21">
         <v>0.37</v>
@@ -2256,13 +2250,13 @@
       <c r="BK10" s="39"/>
       <c r="BL10" s="39"/>
     </row>
-    <row r="11" spans="1:64" s="3" customFormat="1" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="54"/>
       <c r="B11" s="73" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C11" s="64" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D11" s="21">
         <v>0.22</v>
@@ -2332,13 +2326,13 @@
       <c r="BK11" s="39"/>
       <c r="BL11" s="39"/>
     </row>
-    <row r="12" spans="1:64" s="3" customFormat="1" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="53"/>
       <c r="B12" s="73" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C12" s="64" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D12" s="21">
         <v>0</v>
@@ -2416,7 +2410,7 @@
         <v>23</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C13" s="65"/>
       <c r="D13" s="23"/>
@@ -2487,10 +2481,10 @@
     <row r="14" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="54"/>
       <c r="B14" s="74" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C14" s="66" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D14" s="26">
         <v>0</v>
@@ -2566,10 +2560,10 @@
     <row r="15" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="54"/>
       <c r="B15" s="74" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C15" s="66" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D15" s="26">
         <v>0.1</v>
@@ -2644,10 +2638,10 @@
     <row r="16" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="54"/>
       <c r="B16" s="74" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C16" s="66" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D16" s="26">
         <v>0.4</v>
@@ -2720,10 +2714,10 @@
     <row r="17" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="53"/>
       <c r="B17" s="78" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C17" s="66" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D17" s="26">
         <v>0.2</v>
@@ -2797,13 +2791,23 @@
       <c r="BK17" s="39"/>
       <c r="BL17" s="39"/>
     </row>
-    <row r="18" spans="1:64" s="3" customFormat="1" ht="1.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="53"/>
-      <c r="B18" s="74"/>
-      <c r="C18" s="66"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="60"/>
-      <c r="F18" s="60"/>
+      <c r="B18" s="74" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="66" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="26">
+        <v>0</v>
+      </c>
+      <c r="E18" s="60">
+        <v>45018</v>
+      </c>
+      <c r="F18" s="60">
+        <v>45021</v>
+      </c>
       <c r="G18" s="16"/>
       <c r="H18" s="16"/>
       <c r="I18" s="39"/>
@@ -2863,15 +2867,20 @@
       <c r="BK18" s="39"/>
       <c r="BL18" s="39"/>
     </row>
-    <row r="19" spans="1:64" s="3" customFormat="1" ht="38.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="53"/>
-      <c r="B19" s="74"/>
-      <c r="C19" s="66"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="60"/>
-      <c r="F19" s="60"/>
+      <c r="B19" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="67"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="30"/>
       <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
+      <c r="H19" s="16" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
       <c r="I19" s="39"/>
       <c r="J19" s="39"/>
       <c r="K19" s="39"/>
@@ -2888,7 +2897,7 @@
       <c r="V19" s="39"/>
       <c r="W19" s="39"/>
       <c r="X19" s="39"/>
-      <c r="Y19" s="40"/>
+      <c r="Y19" s="39"/>
       <c r="Z19" s="39"/>
       <c r="AA19" s="39"/>
       <c r="AB19" s="39"/>
@@ -2929,25 +2938,28 @@
       <c r="BK19" s="39"/>
       <c r="BL19" s="39"/>
     </row>
-    <row r="20" spans="1:64" s="3" customFormat="1" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="53"/>
-      <c r="B20" s="74" t="s">
-        <v>51</v>
-      </c>
-      <c r="C20" s="66" t="s">
-        <v>31</v>
-      </c>
-      <c r="D20" s="26">
-        <v>0</v>
-      </c>
-      <c r="E20" s="60">
-        <v>45018</v>
-      </c>
-      <c r="F20" s="60">
+      <c r="B20" s="75" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="68" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="E20" s="61">
+        <v>45015</v>
+      </c>
+      <c r="F20" s="61">
         <v>45021</v>
       </c>
       <c r="G20" s="16"/>
-      <c r="H20" s="16"/>
+      <c r="H20" s="16">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
       <c r="I20" s="39"/>
       <c r="J20" s="39"/>
       <c r="K20" s="39"/>
@@ -2964,7 +2976,7 @@
       <c r="V20" s="39"/>
       <c r="W20" s="39"/>
       <c r="X20" s="39"/>
-      <c r="Y20" s="40"/>
+      <c r="Y20" s="39"/>
       <c r="Z20" s="39"/>
       <c r="AA20" s="39"/>
       <c r="AB20" s="39"/>
@@ -3007,18 +3019,23 @@
     </row>
     <row r="21" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="53"/>
-      <c r="B21" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="C21" s="67"/>
-      <c r="D21" s="28"/>
-      <c r="E21" s="29"/>
-      <c r="F21" s="30"/>
+      <c r="B21" s="75" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="68" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" s="31">
+        <v>0</v>
+      </c>
+      <c r="E21" s="61">
+        <v>45020</v>
+      </c>
+      <c r="F21" s="61">
+        <v>45021</v>
+      </c>
       <c r="G21" s="16"/>
-      <c r="H21" s="16" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
+      <c r="H21" s="16"/>
       <c r="I21" s="39"/>
       <c r="J21" s="39"/>
       <c r="K21" s="39"/>
@@ -3079,25 +3096,22 @@
     <row r="22" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="53"/>
       <c r="B22" s="75" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C22" s="68" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D22" s="31">
-        <v>0.5</v>
+        <v>0.22</v>
       </c>
       <c r="E22" s="61">
-        <v>45015</v>
+        <v>45018</v>
       </c>
       <c r="F22" s="61">
         <v>45021</v>
       </c>
       <c r="G22" s="16"/>
-      <c r="H22" s="16">
-        <f t="shared" si="3"/>
-        <v>7</v>
-      </c>
+      <c r="H22" s="16"/>
       <c r="I22" s="39"/>
       <c r="J22" s="39"/>
       <c r="K22" s="39"/>
@@ -3161,19 +3175,22 @@
         <v>38</v>
       </c>
       <c r="C23" s="68" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D23" s="31">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="E23" s="61">
-        <v>45020</v>
+        <v>45017</v>
       </c>
       <c r="F23" s="61">
         <v>45021</v>
       </c>
       <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
+      <c r="H23" s="16">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
       <c r="I23" s="39"/>
       <c r="J23" s="39"/>
       <c r="K23" s="39"/>
@@ -3233,21 +3250,11 @@
     </row>
     <row r="24" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="53"/>
-      <c r="B24" s="75" t="s">
-        <v>37</v>
-      </c>
-      <c r="C24" s="68" t="s">
-        <v>44</v>
-      </c>
-      <c r="D24" s="31">
-        <v>0.22</v>
-      </c>
-      <c r="E24" s="61">
-        <v>45018</v>
-      </c>
-      <c r="F24" s="61">
-        <v>45021</v>
-      </c>
+      <c r="B24" s="76"/>
+      <c r="C24" s="77"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="62"/>
+      <c r="F24" s="62"/>
       <c r="G24" s="16"/>
       <c r="H24" s="16"/>
       <c r="I24" s="39"/>
@@ -3307,28 +3314,15 @@
       <c r="BK24" s="39"/>
       <c r="BL24" s="39"/>
     </row>
-    <row r="25" spans="1:64" s="3" customFormat="1" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="53"/>
-      <c r="B25" s="75" t="s">
-        <v>40</v>
-      </c>
-      <c r="C25" s="68" t="s">
-        <v>44</v>
-      </c>
-      <c r="D25" s="31">
-        <v>0.25</v>
-      </c>
-      <c r="E25" s="61">
-        <v>45017</v>
-      </c>
-      <c r="F25" s="61">
-        <v>45021</v>
-      </c>
+      <c r="B25" s="76"/>
+      <c r="C25" s="77"/>
+      <c r="D25" s="32"/>
+      <c r="E25" s="62"/>
+      <c r="F25" s="62"/>
       <c r="G25" s="16"/>
-      <c r="H25" s="16">
-        <f t="shared" si="3"/>
-        <v>5</v>
-      </c>
+      <c r="H25" s="16"/>
       <c r="I25" s="39"/>
       <c r="J25" s="39"/>
       <c r="K25" s="39"/>
@@ -3386,30 +3380,15 @@
       <c r="BK25" s="39"/>
       <c r="BL25" s="39"/>
     </row>
-    <row r="26" spans="1:64" s="3" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="53"/>
-      <c r="B26" s="75" t="s">
-        <v>36</v>
-      </c>
-      <c r="C26" s="68" t="s">
-        <v>29</v>
-      </c>
-      <c r="D26" s="31">
-        <v>2.5</v>
-      </c>
-      <c r="E26" s="61">
-        <f>F21+1</f>
-        <v>1</v>
-      </c>
-      <c r="F26" s="61">
-        <f t="shared" ref="F26:F34" si="4">E26+1</f>
-        <v>2</v>
-      </c>
+      <c r="B26" s="76"/>
+      <c r="C26" s="77"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="62"/>
+      <c r="F26" s="62"/>
       <c r="G26" s="16"/>
-      <c r="H26" s="16">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
+      <c r="H26" s="16"/>
       <c r="I26" s="39"/>
       <c r="J26" s="39"/>
       <c r="K26" s="39"/>
@@ -3467,915 +3446,81 @@
       <c r="BK26" s="39"/>
       <c r="BL26" s="39"/>
     </row>
-    <row r="27" spans="1:64" s="3" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="53"/>
-      <c r="B27" s="75" t="s">
-        <v>36</v>
-      </c>
-      <c r="C27" s="68" t="s">
-        <v>29</v>
-      </c>
-      <c r="D27" s="31">
-        <v>3.5</v>
-      </c>
-      <c r="E27" s="61" t="e">
-        <f>#REF!+1</f>
-        <v>#REF!</v>
-      </c>
-      <c r="F27" s="61" t="e">
-        <f t="shared" si="4"/>
-        <v>#REF!</v>
-      </c>
-      <c r="G27" s="16"/>
-      <c r="H27" s="16" t="e">
-        <f t="shared" si="3"/>
-        <v>#REF!</v>
-      </c>
-      <c r="I27" s="39"/>
-      <c r="J27" s="39"/>
-      <c r="K27" s="39"/>
-      <c r="L27" s="39"/>
-      <c r="M27" s="39"/>
-      <c r="N27" s="39"/>
-      <c r="O27" s="39"/>
-      <c r="P27" s="39"/>
-      <c r="Q27" s="39"/>
-      <c r="R27" s="39"/>
-      <c r="S27" s="39"/>
-      <c r="T27" s="39"/>
-      <c r="U27" s="39"/>
-      <c r="V27" s="39"/>
-      <c r="W27" s="39"/>
-      <c r="X27" s="39"/>
-      <c r="Y27" s="39"/>
-      <c r="Z27" s="39"/>
-      <c r="AA27" s="39"/>
-      <c r="AB27" s="39"/>
-      <c r="AC27" s="39"/>
-      <c r="AD27" s="39"/>
-      <c r="AE27" s="39"/>
-      <c r="AF27" s="39"/>
-      <c r="AG27" s="39"/>
-      <c r="AH27" s="39"/>
-      <c r="AI27" s="39"/>
-      <c r="AJ27" s="39"/>
-      <c r="AK27" s="39"/>
-      <c r="AL27" s="39"/>
-      <c r="AM27" s="39"/>
-      <c r="AN27" s="39"/>
-      <c r="AO27" s="39"/>
-      <c r="AP27" s="39"/>
-      <c r="AQ27" s="39"/>
-      <c r="AR27" s="39"/>
-      <c r="AS27" s="39"/>
-      <c r="AT27" s="39"/>
-      <c r="AU27" s="39"/>
-      <c r="AV27" s="39"/>
-      <c r="AW27" s="39"/>
-      <c r="AX27" s="39"/>
-      <c r="AY27" s="39"/>
-      <c r="AZ27" s="39"/>
-      <c r="BA27" s="39"/>
-      <c r="BB27" s="39"/>
-      <c r="BC27" s="39"/>
-      <c r="BD27" s="39"/>
-      <c r="BE27" s="39"/>
-      <c r="BF27" s="39"/>
-      <c r="BG27" s="39"/>
-      <c r="BH27" s="39"/>
-      <c r="BI27" s="39"/>
-      <c r="BJ27" s="39"/>
-      <c r="BK27" s="39"/>
-      <c r="BL27" s="39"/>
-    </row>
-    <row r="28" spans="1:64" s="3" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="53"/>
-      <c r="B28" s="75" t="s">
-        <v>36</v>
-      </c>
-      <c r="C28" s="68" t="s">
-        <v>29</v>
-      </c>
-      <c r="D28" s="31">
-        <v>4.5</v>
-      </c>
-      <c r="E28" s="61">
-        <f>F22+1</f>
-        <v>45022</v>
-      </c>
-      <c r="F28" s="61">
-        <f t="shared" si="4"/>
-        <v>45023</v>
-      </c>
-      <c r="G28" s="16"/>
-      <c r="H28" s="16">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="I28" s="39"/>
-      <c r="J28" s="39"/>
-      <c r="K28" s="39"/>
-      <c r="L28" s="39"/>
-      <c r="M28" s="39"/>
-      <c r="N28" s="39"/>
-      <c r="O28" s="39"/>
-      <c r="P28" s="39"/>
-      <c r="Q28" s="39"/>
-      <c r="R28" s="39"/>
-      <c r="S28" s="39"/>
-      <c r="T28" s="39"/>
-      <c r="U28" s="39"/>
-      <c r="V28" s="39"/>
-      <c r="W28" s="39"/>
-      <c r="X28" s="39"/>
-      <c r="Y28" s="39"/>
-      <c r="Z28" s="39"/>
-      <c r="AA28" s="39"/>
-      <c r="AB28" s="39"/>
-      <c r="AC28" s="39"/>
-      <c r="AD28" s="39"/>
-      <c r="AE28" s="39"/>
-      <c r="AF28" s="39"/>
-      <c r="AG28" s="39"/>
-      <c r="AH28" s="39"/>
-      <c r="AI28" s="39"/>
-      <c r="AJ28" s="39"/>
-      <c r="AK28" s="39"/>
-      <c r="AL28" s="39"/>
-      <c r="AM28" s="39"/>
-      <c r="AN28" s="39"/>
-      <c r="AO28" s="39"/>
-      <c r="AP28" s="39"/>
-      <c r="AQ28" s="39"/>
-      <c r="AR28" s="39"/>
-      <c r="AS28" s="39"/>
-      <c r="AT28" s="39"/>
-      <c r="AU28" s="39"/>
-      <c r="AV28" s="39"/>
-      <c r="AW28" s="39"/>
-      <c r="AX28" s="39"/>
-      <c r="AY28" s="39"/>
-      <c r="AZ28" s="39"/>
-      <c r="BA28" s="39"/>
-      <c r="BB28" s="39"/>
-      <c r="BC28" s="39"/>
-      <c r="BD28" s="39"/>
-      <c r="BE28" s="39"/>
-      <c r="BF28" s="39"/>
-      <c r="BG28" s="39"/>
-      <c r="BH28" s="39"/>
-      <c r="BI28" s="39"/>
-      <c r="BJ28" s="39"/>
-      <c r="BK28" s="39"/>
-      <c r="BL28" s="39"/>
-    </row>
-    <row r="29" spans="1:64" s="3" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="53"/>
-      <c r="B29" s="75" t="s">
-        <v>36</v>
-      </c>
-      <c r="C29" s="68" t="s">
-        <v>29</v>
-      </c>
-      <c r="D29" s="31">
-        <v>5.5</v>
-      </c>
-      <c r="E29" s="61">
-        <f>F25+1</f>
-        <v>45022</v>
-      </c>
-      <c r="F29" s="61">
-        <f t="shared" si="4"/>
-        <v>45023</v>
-      </c>
-      <c r="G29" s="16"/>
-      <c r="H29" s="16">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
-      <c r="K29" s="39"/>
-      <c r="L29" s="39"/>
-      <c r="M29" s="39"/>
-      <c r="N29" s="39"/>
-      <c r="O29" s="39"/>
-      <c r="P29" s="39"/>
-      <c r="Q29" s="39"/>
-      <c r="R29" s="39"/>
-      <c r="S29" s="39"/>
-      <c r="T29" s="39"/>
-      <c r="U29" s="39"/>
-      <c r="V29" s="39"/>
-      <c r="W29" s="39"/>
-      <c r="X29" s="39"/>
-      <c r="Y29" s="39"/>
-      <c r="Z29" s="39"/>
-      <c r="AA29" s="39"/>
-      <c r="AB29" s="39"/>
-      <c r="AC29" s="39"/>
-      <c r="AD29" s="39"/>
-      <c r="AE29" s="39"/>
-      <c r="AF29" s="39"/>
-      <c r="AG29" s="39"/>
-      <c r="AH29" s="39"/>
-      <c r="AI29" s="39"/>
-      <c r="AJ29" s="39"/>
-      <c r="AK29" s="39"/>
-      <c r="AL29" s="39"/>
-      <c r="AM29" s="39"/>
-      <c r="AN29" s="39"/>
-      <c r="AO29" s="39"/>
-      <c r="AP29" s="39"/>
-      <c r="AQ29" s="39"/>
-      <c r="AR29" s="39"/>
-      <c r="AS29" s="39"/>
-      <c r="AT29" s="39"/>
-      <c r="AU29" s="39"/>
-      <c r="AV29" s="39"/>
-      <c r="AW29" s="39"/>
-      <c r="AX29" s="39"/>
-      <c r="AY29" s="39"/>
-      <c r="AZ29" s="39"/>
-      <c r="BA29" s="39"/>
-      <c r="BB29" s="39"/>
-      <c r="BC29" s="39"/>
-      <c r="BD29" s="39"/>
-      <c r="BE29" s="39"/>
-      <c r="BF29" s="39"/>
-      <c r="BG29" s="39"/>
-      <c r="BH29" s="39"/>
-      <c r="BI29" s="39"/>
-      <c r="BJ29" s="39"/>
-      <c r="BK29" s="39"/>
-      <c r="BL29" s="39"/>
-    </row>
-    <row r="30" spans="1:64" s="3" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="53"/>
-      <c r="B30" s="75" t="s">
-        <v>36</v>
-      </c>
-      <c r="C30" s="68" t="s">
-        <v>29</v>
-      </c>
-      <c r="D30" s="31">
-        <v>6.5</v>
-      </c>
-      <c r="E30" s="61">
-        <f t="shared" ref="E30:E34" si="5">F26+1</f>
-        <v>3</v>
-      </c>
-      <c r="F30" s="61">
-        <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
-      <c r="G30" s="16"/>
-      <c r="H30" s="16">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="I30" s="39"/>
-      <c r="J30" s="39"/>
-      <c r="K30" s="39"/>
-      <c r="L30" s="39"/>
-      <c r="M30" s="39"/>
-      <c r="N30" s="39"/>
-      <c r="O30" s="39"/>
-      <c r="P30" s="39"/>
-      <c r="Q30" s="39"/>
-      <c r="R30" s="39"/>
-      <c r="S30" s="39"/>
-      <c r="T30" s="39"/>
-      <c r="U30" s="39"/>
-      <c r="V30" s="39"/>
-      <c r="W30" s="39"/>
-      <c r="X30" s="39"/>
-      <c r="Y30" s="39"/>
-      <c r="Z30" s="39"/>
-      <c r="AA30" s="39"/>
-      <c r="AB30" s="39"/>
-      <c r="AC30" s="39"/>
-      <c r="AD30" s="39"/>
-      <c r="AE30" s="39"/>
-      <c r="AF30" s="39"/>
-      <c r="AG30" s="39"/>
-      <c r="AH30" s="39"/>
-      <c r="AI30" s="39"/>
-      <c r="AJ30" s="39"/>
-      <c r="AK30" s="39"/>
-      <c r="AL30" s="39"/>
-      <c r="AM30" s="39"/>
-      <c r="AN30" s="39"/>
-      <c r="AO30" s="39"/>
-      <c r="AP30" s="39"/>
-      <c r="AQ30" s="39"/>
-      <c r="AR30" s="39"/>
-      <c r="AS30" s="39"/>
-      <c r="AT30" s="39"/>
-      <c r="AU30" s="39"/>
-      <c r="AV30" s="39"/>
-      <c r="AW30" s="39"/>
-      <c r="AX30" s="39"/>
-      <c r="AY30" s="39"/>
-      <c r="AZ30" s="39"/>
-      <c r="BA30" s="39"/>
-      <c r="BB30" s="39"/>
-      <c r="BC30" s="39"/>
-      <c r="BD30" s="39"/>
-      <c r="BE30" s="39"/>
-      <c r="BF30" s="39"/>
-      <c r="BG30" s="39"/>
-      <c r="BH30" s="39"/>
-      <c r="BI30" s="39"/>
-      <c r="BJ30" s="39"/>
-      <c r="BK30" s="39"/>
-      <c r="BL30" s="39"/>
-    </row>
-    <row r="31" spans="1:64" s="3" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="53"/>
-      <c r="B31" s="75" t="s">
-        <v>36</v>
-      </c>
-      <c r="C31" s="68" t="s">
-        <v>29</v>
-      </c>
-      <c r="D31" s="31">
-        <v>7.5</v>
-      </c>
-      <c r="E31" s="61" t="e">
-        <f t="shared" si="5"/>
-        <v>#REF!</v>
-      </c>
-      <c r="F31" s="61" t="e">
-        <f t="shared" si="4"/>
-        <v>#REF!</v>
-      </c>
-      <c r="G31" s="16"/>
-      <c r="H31" s="16" t="e">
-        <f t="shared" si="3"/>
-        <v>#REF!</v>
-      </c>
-      <c r="I31" s="39"/>
-      <c r="J31" s="39"/>
-      <c r="K31" s="39"/>
-      <c r="L31" s="39"/>
-      <c r="M31" s="39"/>
-      <c r="N31" s="39"/>
-      <c r="O31" s="39"/>
-      <c r="P31" s="39"/>
-      <c r="Q31" s="39"/>
-      <c r="R31" s="39"/>
-      <c r="S31" s="39"/>
-      <c r="T31" s="39"/>
-      <c r="U31" s="39"/>
-      <c r="V31" s="39"/>
-      <c r="W31" s="39"/>
-      <c r="X31" s="39"/>
-      <c r="Y31" s="39"/>
-      <c r="Z31" s="39"/>
-      <c r="AA31" s="39"/>
-      <c r="AB31" s="39"/>
-      <c r="AC31" s="39"/>
-      <c r="AD31" s="39"/>
-      <c r="AE31" s="39"/>
-      <c r="AF31" s="39"/>
-      <c r="AG31" s="39"/>
-      <c r="AH31" s="39"/>
-      <c r="AI31" s="39"/>
-      <c r="AJ31" s="39"/>
-      <c r="AK31" s="39"/>
-      <c r="AL31" s="39"/>
-      <c r="AM31" s="39"/>
-      <c r="AN31" s="39"/>
-      <c r="AO31" s="39"/>
-      <c r="AP31" s="39"/>
-      <c r="AQ31" s="39"/>
-      <c r="AR31" s="39"/>
-      <c r="AS31" s="39"/>
-      <c r="AT31" s="39"/>
-      <c r="AU31" s="39"/>
-      <c r="AV31" s="39"/>
-      <c r="AW31" s="39"/>
-      <c r="AX31" s="39"/>
-      <c r="AY31" s="39"/>
-      <c r="AZ31" s="39"/>
-      <c r="BA31" s="39"/>
-      <c r="BB31" s="39"/>
-      <c r="BC31" s="39"/>
-      <c r="BD31" s="39"/>
-      <c r="BE31" s="39"/>
-      <c r="BF31" s="39"/>
-      <c r="BG31" s="39"/>
-      <c r="BH31" s="39"/>
-      <c r="BI31" s="39"/>
-      <c r="BJ31" s="39"/>
-      <c r="BK31" s="39"/>
-      <c r="BL31" s="39"/>
-    </row>
-    <row r="32" spans="1:64" s="3" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="53"/>
-      <c r="B32" s="75" t="s">
-        <v>36</v>
-      </c>
-      <c r="C32" s="68" t="s">
-        <v>29</v>
-      </c>
-      <c r="D32" s="31">
-        <v>8.5</v>
-      </c>
-      <c r="E32" s="61">
-        <f t="shared" si="5"/>
-        <v>45024</v>
-      </c>
-      <c r="F32" s="61">
-        <f t="shared" si="4"/>
-        <v>45025</v>
-      </c>
-      <c r="G32" s="16"/>
-      <c r="H32" s="16">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="I32" s="39"/>
-      <c r="J32" s="39"/>
-      <c r="K32" s="39"/>
-      <c r="L32" s="39"/>
-      <c r="M32" s="39"/>
-      <c r="N32" s="39"/>
-      <c r="O32" s="39"/>
-      <c r="P32" s="39"/>
-      <c r="Q32" s="39"/>
-      <c r="R32" s="39"/>
-      <c r="S32" s="39"/>
-      <c r="T32" s="39"/>
-      <c r="U32" s="39"/>
-      <c r="V32" s="39"/>
-      <c r="W32" s="39"/>
-      <c r="X32" s="39"/>
-      <c r="Y32" s="39"/>
-      <c r="Z32" s="39"/>
-      <c r="AA32" s="39"/>
-      <c r="AB32" s="39"/>
-      <c r="AC32" s="39"/>
-      <c r="AD32" s="39"/>
-      <c r="AE32" s="39"/>
-      <c r="AF32" s="39"/>
-      <c r="AG32" s="39"/>
-      <c r="AH32" s="39"/>
-      <c r="AI32" s="39"/>
-      <c r="AJ32" s="39"/>
-      <c r="AK32" s="39"/>
-      <c r="AL32" s="39"/>
-      <c r="AM32" s="39"/>
-      <c r="AN32" s="39"/>
-      <c r="AO32" s="39"/>
-      <c r="AP32" s="39"/>
-      <c r="AQ32" s="39"/>
-      <c r="AR32" s="39"/>
-      <c r="AS32" s="39"/>
-      <c r="AT32" s="39"/>
-      <c r="AU32" s="39"/>
-      <c r="AV32" s="39"/>
-      <c r="AW32" s="39"/>
-      <c r="AX32" s="39"/>
-      <c r="AY32" s="39"/>
-      <c r="AZ32" s="39"/>
-      <c r="BA32" s="39"/>
-      <c r="BB32" s="39"/>
-      <c r="BC32" s="39"/>
-      <c r="BD32" s="39"/>
-      <c r="BE32" s="39"/>
-      <c r="BF32" s="39"/>
-      <c r="BG32" s="39"/>
-      <c r="BH32" s="39"/>
-      <c r="BI32" s="39"/>
-      <c r="BJ32" s="39"/>
-      <c r="BK32" s="39"/>
-      <c r="BL32" s="39"/>
-    </row>
-    <row r="33" spans="1:64" s="3" customFormat="1" ht="1.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="53"/>
-      <c r="B33" s="75" t="s">
-        <v>36</v>
-      </c>
-      <c r="C33" s="68" t="s">
-        <v>29</v>
-      </c>
-      <c r="D33" s="31">
-        <v>9.5</v>
-      </c>
-      <c r="E33" s="61">
-        <f t="shared" si="5"/>
-        <v>45024</v>
-      </c>
-      <c r="F33" s="61">
-        <f t="shared" si="4"/>
-        <v>45025</v>
-      </c>
-      <c r="G33" s="16"/>
-      <c r="H33" s="16">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="I33" s="39"/>
-      <c r="J33" s="39"/>
-      <c r="K33" s="39"/>
-      <c r="L33" s="39"/>
-      <c r="M33" s="39"/>
-      <c r="N33" s="39"/>
-      <c r="O33" s="39"/>
-      <c r="P33" s="39"/>
-      <c r="Q33" s="39"/>
-      <c r="R33" s="39"/>
-      <c r="S33" s="39"/>
-      <c r="T33" s="39"/>
-      <c r="U33" s="39"/>
-      <c r="V33" s="39"/>
-      <c r="W33" s="39"/>
-      <c r="X33" s="39"/>
-      <c r="Y33" s="39"/>
-      <c r="Z33" s="39"/>
-      <c r="AA33" s="39"/>
-      <c r="AB33" s="39"/>
-      <c r="AC33" s="39"/>
-      <c r="AD33" s="39"/>
-      <c r="AE33" s="39"/>
-      <c r="AF33" s="39"/>
-      <c r="AG33" s="39"/>
-      <c r="AH33" s="39"/>
-      <c r="AI33" s="39"/>
-      <c r="AJ33" s="39"/>
-      <c r="AK33" s="39"/>
-      <c r="AL33" s="39"/>
-      <c r="AM33" s="39"/>
-      <c r="AN33" s="39"/>
-      <c r="AO33" s="39"/>
-      <c r="AP33" s="39"/>
-      <c r="AQ33" s="39"/>
-      <c r="AR33" s="39"/>
-      <c r="AS33" s="39"/>
-      <c r="AT33" s="39"/>
-      <c r="AU33" s="39"/>
-      <c r="AV33" s="39"/>
-      <c r="AW33" s="39"/>
-      <c r="AX33" s="39"/>
-      <c r="AY33" s="39"/>
-      <c r="AZ33" s="39"/>
-      <c r="BA33" s="39"/>
-      <c r="BB33" s="39"/>
-      <c r="BC33" s="39"/>
-      <c r="BD33" s="39"/>
-      <c r="BE33" s="39"/>
-      <c r="BF33" s="39"/>
-      <c r="BG33" s="39"/>
-      <c r="BH33" s="39"/>
-      <c r="BI33" s="39"/>
-      <c r="BJ33" s="39"/>
-      <c r="BK33" s="39"/>
-      <c r="BL33" s="39"/>
-    </row>
-    <row r="34" spans="1:64" s="3" customFormat="1" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="53"/>
-      <c r="B34" s="75"/>
-      <c r="C34" s="68"/>
-      <c r="D34" s="31"/>
-      <c r="E34" s="61"/>
-      <c r="F34" s="61"/>
-      <c r="G34" s="16"/>
-      <c r="H34" s="16" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="I34" s="39"/>
-      <c r="J34" s="39"/>
-      <c r="K34" s="39"/>
-      <c r="L34" s="39"/>
-      <c r="M34" s="39"/>
-      <c r="N34" s="39"/>
-      <c r="O34" s="39"/>
-      <c r="P34" s="39"/>
-      <c r="Q34" s="39"/>
-      <c r="R34" s="39"/>
-      <c r="S34" s="39"/>
-      <c r="T34" s="39"/>
-      <c r="U34" s="39"/>
-      <c r="V34" s="39"/>
-      <c r="W34" s="39"/>
-      <c r="X34" s="39"/>
-      <c r="Y34" s="39"/>
-      <c r="Z34" s="39"/>
-      <c r="AA34" s="39"/>
-      <c r="AB34" s="39"/>
-      <c r="AC34" s="39"/>
-      <c r="AD34" s="39"/>
-      <c r="AE34" s="39"/>
-      <c r="AF34" s="39"/>
-      <c r="AG34" s="39"/>
-      <c r="AH34" s="39"/>
-      <c r="AI34" s="39"/>
-      <c r="AJ34" s="39"/>
-      <c r="AK34" s="39"/>
-      <c r="AL34" s="39"/>
-      <c r="AM34" s="39"/>
-      <c r="AN34" s="39"/>
-      <c r="AO34" s="39"/>
-      <c r="AP34" s="39"/>
-      <c r="AQ34" s="39"/>
-      <c r="AR34" s="39"/>
-      <c r="AS34" s="39"/>
-      <c r="AT34" s="39"/>
-      <c r="AU34" s="39"/>
-      <c r="AV34" s="39"/>
-      <c r="AW34" s="39"/>
-      <c r="AX34" s="39"/>
-      <c r="AY34" s="39"/>
-      <c r="AZ34" s="39"/>
-      <c r="BA34" s="39"/>
-      <c r="BB34" s="39"/>
-      <c r="BC34" s="39"/>
-      <c r="BD34" s="39"/>
-      <c r="BE34" s="39"/>
-      <c r="BF34" s="39"/>
-      <c r="BG34" s="39"/>
-      <c r="BH34" s="39"/>
-      <c r="BI34" s="39"/>
-      <c r="BJ34" s="39"/>
-      <c r="BK34" s="39"/>
-      <c r="BL34" s="39"/>
-    </row>
-    <row r="35" spans="1:64" s="3" customFormat="1" ht="28.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="53"/>
-      <c r="B35" s="76"/>
-      <c r="C35" s="77"/>
-      <c r="D35" s="32"/>
-      <c r="E35" s="62"/>
-      <c r="F35" s="62"/>
-      <c r="G35" s="16"/>
-      <c r="H35" s="16"/>
-      <c r="I35" s="39"/>
-      <c r="J35" s="39"/>
-      <c r="K35" s="39"/>
-      <c r="L35" s="39"/>
-      <c r="M35" s="39"/>
-      <c r="N35" s="39"/>
-      <c r="O35" s="39"/>
-      <c r="P35" s="39"/>
-      <c r="Q35" s="39"/>
-      <c r="R35" s="39"/>
-      <c r="S35" s="39"/>
-      <c r="T35" s="39"/>
-      <c r="U35" s="39"/>
-      <c r="V35" s="39"/>
-      <c r="W35" s="39"/>
-      <c r="X35" s="39"/>
-      <c r="Y35" s="39"/>
-      <c r="Z35" s="39"/>
-      <c r="AA35" s="39"/>
-      <c r="AB35" s="39"/>
-      <c r="AC35" s="39"/>
-      <c r="AD35" s="39"/>
-      <c r="AE35" s="39"/>
-      <c r="AF35" s="39"/>
-      <c r="AG35" s="39"/>
-      <c r="AH35" s="39"/>
-      <c r="AI35" s="39"/>
-      <c r="AJ35" s="39"/>
-      <c r="AK35" s="39"/>
-      <c r="AL35" s="39"/>
-      <c r="AM35" s="39"/>
-      <c r="AN35" s="39"/>
-      <c r="AO35" s="39"/>
-      <c r="AP35" s="39"/>
-      <c r="AQ35" s="39"/>
-      <c r="AR35" s="39"/>
-      <c r="AS35" s="39"/>
-      <c r="AT35" s="39"/>
-      <c r="AU35" s="39"/>
-      <c r="AV35" s="39"/>
-      <c r="AW35" s="39"/>
-      <c r="AX35" s="39"/>
-      <c r="AY35" s="39"/>
-      <c r="AZ35" s="39"/>
-      <c r="BA35" s="39"/>
-      <c r="BB35" s="39"/>
-      <c r="BC35" s="39"/>
-      <c r="BD35" s="39"/>
-      <c r="BE35" s="39"/>
-      <c r="BF35" s="39"/>
-      <c r="BG35" s="39"/>
-      <c r="BH35" s="39"/>
-      <c r="BI35" s="39"/>
-      <c r="BJ35" s="39"/>
-      <c r="BK35" s="39"/>
-      <c r="BL35" s="39"/>
-    </row>
-    <row r="36" spans="1:64" s="3" customFormat="1" ht="33" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="53"/>
-      <c r="B36" s="76"/>
-      <c r="C36" s="77"/>
-      <c r="D36" s="32"/>
-      <c r="E36" s="62"/>
-      <c r="F36" s="62"/>
-      <c r="G36" s="16"/>
-      <c r="H36" s="16"/>
-      <c r="I36" s="39"/>
-      <c r="J36" s="39"/>
-      <c r="K36" s="39"/>
-      <c r="L36" s="39"/>
-      <c r="M36" s="39"/>
-      <c r="N36" s="39"/>
-      <c r="O36" s="39"/>
-      <c r="P36" s="39"/>
-      <c r="Q36" s="39"/>
-      <c r="R36" s="39"/>
-      <c r="S36" s="39"/>
-      <c r="T36" s="39"/>
-      <c r="U36" s="39"/>
-      <c r="V36" s="39"/>
-      <c r="W36" s="39"/>
-      <c r="X36" s="39"/>
-      <c r="Y36" s="39"/>
-      <c r="Z36" s="39"/>
-      <c r="AA36" s="39"/>
-      <c r="AB36" s="39"/>
-      <c r="AC36" s="39"/>
-      <c r="AD36" s="39"/>
-      <c r="AE36" s="39"/>
-      <c r="AF36" s="39"/>
-      <c r="AG36" s="39"/>
-      <c r="AH36" s="39"/>
-      <c r="AI36" s="39"/>
-      <c r="AJ36" s="39"/>
-      <c r="AK36" s="39"/>
-      <c r="AL36" s="39"/>
-      <c r="AM36" s="39"/>
-      <c r="AN36" s="39"/>
-      <c r="AO36" s="39"/>
-      <c r="AP36" s="39"/>
-      <c r="AQ36" s="39"/>
-      <c r="AR36" s="39"/>
-      <c r="AS36" s="39"/>
-      <c r="AT36" s="39"/>
-      <c r="AU36" s="39"/>
-      <c r="AV36" s="39"/>
-      <c r="AW36" s="39"/>
-      <c r="AX36" s="39"/>
-      <c r="AY36" s="39"/>
-      <c r="AZ36" s="39"/>
-      <c r="BA36" s="39"/>
-      <c r="BB36" s="39"/>
-      <c r="BC36" s="39"/>
-      <c r="BD36" s="39"/>
-      <c r="BE36" s="39"/>
-      <c r="BF36" s="39"/>
-      <c r="BG36" s="39"/>
-      <c r="BH36" s="39"/>
-      <c r="BI36" s="39"/>
-      <c r="BJ36" s="39"/>
-      <c r="BK36" s="39"/>
-      <c r="BL36" s="39"/>
-    </row>
-    <row r="37" spans="1:64" s="3" customFormat="1" ht="1.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="53"/>
-      <c r="B37" s="76"/>
-      <c r="C37" s="77"/>
-      <c r="D37" s="32"/>
-      <c r="E37" s="62"/>
-      <c r="F37" s="62"/>
-      <c r="G37" s="16"/>
-      <c r="H37" s="16"/>
-      <c r="I37" s="39"/>
-      <c r="J37" s="39"/>
-      <c r="K37" s="39"/>
-      <c r="L37" s="39"/>
-      <c r="M37" s="39"/>
-      <c r="N37" s="39"/>
-      <c r="O37" s="39"/>
-      <c r="P37" s="39"/>
-      <c r="Q37" s="39"/>
-      <c r="R37" s="39"/>
-      <c r="S37" s="39"/>
-      <c r="T37" s="39"/>
-      <c r="U37" s="39"/>
-      <c r="V37" s="39"/>
-      <c r="W37" s="39"/>
-      <c r="X37" s="39"/>
-      <c r="Y37" s="39"/>
-      <c r="Z37" s="39"/>
-      <c r="AA37" s="39"/>
-      <c r="AB37" s="39"/>
-      <c r="AC37" s="39"/>
-      <c r="AD37" s="39"/>
-      <c r="AE37" s="39"/>
-      <c r="AF37" s="39"/>
-      <c r="AG37" s="39"/>
-      <c r="AH37" s="39"/>
-      <c r="AI37" s="39"/>
-      <c r="AJ37" s="39"/>
-      <c r="AK37" s="39"/>
-      <c r="AL37" s="39"/>
-      <c r="AM37" s="39"/>
-      <c r="AN37" s="39"/>
-      <c r="AO37" s="39"/>
-      <c r="AP37" s="39"/>
-      <c r="AQ37" s="39"/>
-      <c r="AR37" s="39"/>
-      <c r="AS37" s="39"/>
-      <c r="AT37" s="39"/>
-      <c r="AU37" s="39"/>
-      <c r="AV37" s="39"/>
-      <c r="AW37" s="39"/>
-      <c r="AX37" s="39"/>
-      <c r="AY37" s="39"/>
-      <c r="AZ37" s="39"/>
-      <c r="BA37" s="39"/>
-      <c r="BB37" s="39"/>
-      <c r="BC37" s="39"/>
-      <c r="BD37" s="39"/>
-      <c r="BE37" s="39"/>
-      <c r="BF37" s="39"/>
-      <c r="BG37" s="39"/>
-      <c r="BH37" s="39"/>
-      <c r="BI37" s="39"/>
-      <c r="BJ37" s="39"/>
-      <c r="BK37" s="39"/>
-      <c r="BL37" s="39"/>
-    </row>
-    <row r="38" spans="1:64" s="3" customFormat="1" ht="1.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="54"/>
-      <c r="B38" s="33"/>
-      <c r="C38" s="34"/>
-      <c r="D38" s="35"/>
-      <c r="E38" s="36"/>
-      <c r="F38" s="37"/>
-      <c r="G38" s="38"/>
-      <c r="H38" s="38"/>
-      <c r="I38" s="41"/>
-      <c r="J38" s="41"/>
-      <c r="K38" s="41"/>
-      <c r="L38" s="41"/>
-      <c r="M38" s="41"/>
-      <c r="N38" s="41"/>
-      <c r="O38" s="41"/>
-      <c r="P38" s="41"/>
-      <c r="Q38" s="41"/>
-      <c r="R38" s="41"/>
-      <c r="S38" s="41"/>
-      <c r="T38" s="41"/>
-      <c r="U38" s="41"/>
-      <c r="V38" s="41"/>
-      <c r="W38" s="41"/>
-      <c r="X38" s="41"/>
-      <c r="Y38" s="41"/>
-      <c r="Z38" s="41"/>
-      <c r="AA38" s="41"/>
-      <c r="AB38" s="41"/>
-      <c r="AC38" s="41"/>
-      <c r="AD38" s="41"/>
-      <c r="AE38" s="41"/>
-      <c r="AF38" s="41"/>
-      <c r="AG38" s="41"/>
-      <c r="AH38" s="41"/>
-      <c r="AI38" s="41"/>
-      <c r="AJ38" s="41"/>
-      <c r="AK38" s="41"/>
-      <c r="AL38" s="41"/>
-      <c r="AM38" s="41"/>
-      <c r="AN38" s="41"/>
-      <c r="AO38" s="41"/>
-      <c r="AP38" s="41"/>
-      <c r="AQ38" s="41"/>
-      <c r="AR38" s="41"/>
-      <c r="AS38" s="41"/>
-      <c r="AT38" s="41"/>
-      <c r="AU38" s="41"/>
-      <c r="AV38" s="41"/>
-      <c r="AW38" s="41"/>
-      <c r="AX38" s="41"/>
-      <c r="AY38" s="41"/>
-      <c r="AZ38" s="41"/>
-      <c r="BA38" s="41"/>
-      <c r="BB38" s="41"/>
-      <c r="BC38" s="41"/>
-      <c r="BD38" s="41"/>
-      <c r="BE38" s="41"/>
-      <c r="BF38" s="41"/>
-      <c r="BG38" s="41"/>
-      <c r="BH38" s="41"/>
-      <c r="BI38" s="41"/>
-      <c r="BJ38" s="41"/>
-      <c r="BK38" s="41"/>
-      <c r="BL38" s="41"/>
-    </row>
-    <row r="39" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G39" s="6"/>
-    </row>
-    <row r="40" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C40" s="14"/>
-      <c r="F40" s="55"/>
-    </row>
-    <row r="41" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C41" s="15"/>
+    <row r="27" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="54"/>
+      <c r="B27" s="33"/>
+      <c r="C27" s="34"/>
+      <c r="D27" s="35"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="38"/>
+      <c r="I27" s="41"/>
+      <c r="J27" s="41"/>
+      <c r="K27" s="41"/>
+      <c r="L27" s="41"/>
+      <c r="M27" s="41"/>
+      <c r="N27" s="41"/>
+      <c r="O27" s="41"/>
+      <c r="P27" s="41"/>
+      <c r="Q27" s="41"/>
+      <c r="R27" s="41"/>
+      <c r="S27" s="41"/>
+      <c r="T27" s="41"/>
+      <c r="U27" s="41"/>
+      <c r="V27" s="41"/>
+      <c r="W27" s="41"/>
+      <c r="X27" s="41"/>
+      <c r="Y27" s="41"/>
+      <c r="Z27" s="41"/>
+      <c r="AA27" s="41"/>
+      <c r="AB27" s="41"/>
+      <c r="AC27" s="41"/>
+      <c r="AD27" s="41"/>
+      <c r="AE27" s="41"/>
+      <c r="AF27" s="41"/>
+      <c r="AG27" s="41"/>
+      <c r="AH27" s="41"/>
+      <c r="AI27" s="41"/>
+      <c r="AJ27" s="41"/>
+      <c r="AK27" s="41"/>
+      <c r="AL27" s="41"/>
+      <c r="AM27" s="41"/>
+      <c r="AN27" s="41"/>
+      <c r="AO27" s="41"/>
+      <c r="AP27" s="41"/>
+      <c r="AQ27" s="41"/>
+      <c r="AR27" s="41"/>
+      <c r="AS27" s="41"/>
+      <c r="AT27" s="41"/>
+      <c r="AU27" s="41"/>
+      <c r="AV27" s="41"/>
+      <c r="AW27" s="41"/>
+      <c r="AX27" s="41"/>
+      <c r="AY27" s="41"/>
+      <c r="AZ27" s="41"/>
+      <c r="BA27" s="41"/>
+      <c r="BB27" s="41"/>
+      <c r="BC27" s="41"/>
+      <c r="BD27" s="41"/>
+      <c r="BE27" s="41"/>
+      <c r="BF27" s="41"/>
+      <c r="BG27" s="41"/>
+      <c r="BH27" s="41"/>
+      <c r="BI27" s="41"/>
+      <c r="BJ27" s="41"/>
+      <c r="BK27" s="41"/>
+      <c r="BL27" s="41"/>
+    </row>
+    <row r="28" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G28" s="6"/>
+    </row>
+    <row r="29" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C29" s="14"/>
+      <c r="F29" s="55"/>
+    </row>
+    <row r="30" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C30" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -4394,7 +3539,7 @@
     <mergeCell ref="L3:P3"/>
     <mergeCell ref="R3:V3"/>
   </mergeCells>
-  <conditionalFormatting sqref="D7:D38">
+  <conditionalFormatting sqref="D7:D27">
     <cfRule type="dataBar" priority="14">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -4408,12 +3553,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I5:BL38">
+  <conditionalFormatting sqref="I5:BL27">
     <cfRule type="expression" dxfId="2" priority="33">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I7:BL38">
+  <conditionalFormatting sqref="I7:BL27">
     <cfRule type="expression" dxfId="1" priority="27">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
@@ -4448,7 +3593,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D7:D38</xm:sqref>
+          <xm:sqref>D7:D27</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>